<commit_message>
editing for the reruns
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 8 Permutations/Trial 8 Permutation_no-constants_Summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 8 Permutations/Trial 8 Permutation_no-constants_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\Travel-Conferences\BOSC_ISMB_2025\trial 8 permutations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0149E945-14F4-44B6-8102-BB767643ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{153AE62B-9851-4887-A1D4-678FAF962D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="787" firstSheet="14" activeTab="2" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20784" windowHeight="11328" tabRatio="787" activeTab="1" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
   </bookViews>
   <sheets>
     <sheet name="No Constants" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="26">
   <si>
     <t>Parameter</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reran on lab computer for consistancy </t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -236,8 +239,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,35 +402,35 @@
                 <c:pt idx="6">
                   <c:v>8.07</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>8.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>8.19</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.00">
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>8.06</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.00">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>8.1</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.00">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>8.08</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>8.17</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>8.23</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="0.00">
+                <c:pt idx="14" formatCode="0.00">
                   <c:v>8.14</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00">
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>8.1199999999999992</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0.00">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>8.18</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00">
-                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>8.1300000000000008</c:v>
@@ -479,37 +484,37 @@
                   <c:v>0.12463458598619642</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.17238004932911505</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.22579166495981087</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.27286498652861313</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.36227442272078858</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.53628400644574326</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.54083169304672596</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.6030306303351427</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.74922399674353879</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.7632158533220309</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.0601366671880055</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.2345762179032729</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6826918202478027</c:v>
+                  <c:v>1.6333560392801805</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>2.2486088556715709</c:v>
@@ -671,6 +676,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -678,7 +684,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1085,7 +1090,7 @@
                   <c:v>0.12463458598619642</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2345762179032729</c:v>
+                  <c:v>0.17238004932911505</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7.3570491299070548E-2</c:v>
@@ -1130,7 +1135,7 @@
                   <c:v>0.36227442272078858</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.6826918202478027</c:v>
+                  <c:v>1.6333560392801805</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>6.0862391056363874E-2</c:v>
@@ -1294,6 +1299,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1301,7 +1307,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2825,21 +2830,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7478D67-BA7D-48FA-92AF-8000621A116E}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+    <sheetView topLeftCell="A7" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -2879,7 +2884,7 @@
         <v>7.9064243696657428E-9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8.01</v>
       </c>
@@ -2899,15 +2904,15 @@
         <v>1.1490204021044756E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>8.02</v>
       </c>
       <c r="B4" s="11">
-        <v>1.2345762179032729</v>
+        <v>0.17238004932911505</v>
       </c>
       <c r="C4" s="11">
-        <v>1.4103999578405046E-9</v>
+        <v>1.1307916401083287E-9</v>
       </c>
       <c r="E4" s="1">
         <v>8.0399999999999991</v>
@@ -2919,7 +2924,7 @@
         <v>8.9091668745862933E-10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8.0299999999999994</v>
       </c>
@@ -2939,7 +2944,7 @@
         <v>1.7904110275793348E-10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>8.0399999999999991</v>
       </c>
@@ -2959,7 +2964,7 @@
         <v>2.9712204569654842E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8.0500000000000007</v>
       </c>
@@ -2979,7 +2984,7 @@
         <v>8.7237338019770477E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8.06</v>
       </c>
@@ -2999,7 +3004,7 @@
         <v>1.9136102498212524E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8.07</v>
       </c>
@@ -3009,17 +3014,17 @@
       <c r="C9">
         <v>1.9136102498212524E-10</v>
       </c>
-      <c r="E9">
-        <v>8.19</v>
-      </c>
-      <c r="F9">
-        <v>0.22579166495981087</v>
-      </c>
-      <c r="G9">
-        <v>5.5196531199937079E-8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="10">
+        <v>8.02</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.17238004932911505</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1.1307916401083287E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8.08</v>
       </c>
@@ -3029,17 +3034,17 @@
       <c r="C10">
         <v>4.4705591269123412E-10</v>
       </c>
-      <c r="E10" s="1">
-        <v>8.06</v>
+      <c r="E10">
+        <v>8.19</v>
       </c>
       <c r="F10">
-        <v>0.27286498652861313</v>
+        <v>0.22579166495981087</v>
       </c>
       <c r="G10">
-        <v>8.4890169354810502E-10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5.5196531199937079E-8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8.09</v>
       </c>
@@ -3050,16 +3055,16 @@
         <v>1.220527454176325E-9</v>
       </c>
       <c r="E11" s="1">
-        <v>8.1</v>
+        <v>8.06</v>
       </c>
       <c r="F11">
-        <v>0.36227442272078858</v>
+        <v>0.27286498652861313</v>
       </c>
       <c r="G11">
-        <v>1.5112308569915994E-10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.4890169354810502E-10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8.1</v>
       </c>
@@ -3070,16 +3075,16 @@
         <v>1.5112308569915994E-10</v>
       </c>
       <c r="E12" s="1">
-        <v>8.08</v>
+        <v>8.1</v>
       </c>
       <c r="F12">
-        <v>0.53628400644574326</v>
+        <v>0.36227442272078858</v>
       </c>
       <c r="G12">
-        <v>4.4705591269123412E-10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1.5112308569915994E-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8.11</v>
       </c>
@@ -3089,17 +3094,17 @@
       <c r="C13">
         <v>1.1861010101689067E-8</v>
       </c>
-      <c r="E13">
-        <v>8.17</v>
+      <c r="E13" s="1">
+        <v>8.08</v>
       </c>
       <c r="F13">
-        <v>0.54083169304672596</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4.0999506860738474E-8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.53628400644574326</v>
+      </c>
+      <c r="G13">
+        <v>4.4705591269123412E-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8.1199999999999992</v>
       </c>
@@ -3110,36 +3115,36 @@
         <v>1.864762686649549E-8</v>
       </c>
       <c r="E14">
-        <v>8.23</v>
+        <v>8.17</v>
       </c>
       <c r="F14">
-        <v>0.6030306303351427</v>
-      </c>
-      <c r="G14">
-        <v>2.2654785451594287E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.54083169304672596</v>
+      </c>
+      <c r="G14" s="15">
+        <v>4.0999506860738474E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>8.1300000000000008</v>
       </c>
       <c r="B15" s="11">
-        <v>1.6826918202478027</v>
-      </c>
-      <c r="C15" s="11">
-        <v>1.0494704587924837E-9</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8.14</v>
+        <v>1.6333560392801805</v>
+      </c>
+      <c r="C15" s="15">
+        <v>5.4501942678475027E-9</v>
+      </c>
+      <c r="E15">
+        <v>8.23</v>
       </c>
       <c r="F15">
-        <v>0.74922399674353879</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1.0259712564787353E-10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.6030306303351427</v>
+      </c>
+      <c r="G15">
+        <v>2.2654785451594287E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>8.14</v>
       </c>
@@ -3150,16 +3155,16 @@
         <v>1.0259712564787353E-10</v>
       </c>
       <c r="E16" s="1">
-        <v>8.1199999999999992</v>
+        <v>8.14</v>
       </c>
       <c r="F16">
-        <v>0.7632158533220309</v>
-      </c>
-      <c r="G16">
-        <v>1.864762686649549E-8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.74922399674353879</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1.0259712564787353E-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8.15</v>
       </c>
@@ -3170,16 +3175,16 @@
         <v>4.3395007995374765E-8</v>
       </c>
       <c r="E17" s="1">
-        <v>8.18</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="F17">
-        <v>1.0601366671880055</v>
+        <v>0.7632158533220309</v>
       </c>
       <c r="G17">
-        <v>2.4703818590741491E-9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.864762686649549E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>8.16</v>
       </c>
@@ -3189,17 +3194,17 @@
       <c r="C18">
         <v>1.7904110275793348E-10</v>
       </c>
-      <c r="E18" s="10">
-        <v>8.02</v>
-      </c>
-      <c r="F18" s="11">
-        <v>1.2345762179032729</v>
-      </c>
-      <c r="G18" s="11">
-        <v>1.4103999578405046E-9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>8.18</v>
+      </c>
+      <c r="F18">
+        <v>1.0601366671880055</v>
+      </c>
+      <c r="G18">
+        <v>2.4703818590741491E-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8.17</v>
       </c>
@@ -3213,13 +3218,13 @@
         <v>8.1300000000000008</v>
       </c>
       <c r="F19" s="11">
-        <v>1.6826918202478027</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1.0494704587924837E-9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.6333560392801805</v>
+      </c>
+      <c r="G19" s="15">
+        <v>5.4501942678475027E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>8.18</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>3.6877599043628843E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8.19</v>
       </c>
@@ -3259,7 +3264,7 @@
         <v>1.220612791800669E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>8.1999999999999993</v>
       </c>
@@ -3279,7 +3284,7 @@
         <v>3.2114771968466949E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8.2100000000000009</v>
       </c>
@@ -3299,7 +3304,7 @@
         <v>1.1861010101689067E-8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>8.2200000000000006</v>
       </c>
@@ -3319,7 +3324,7 @@
         <v>1.220527454176325E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8.23</v>
       </c>
@@ -3339,25 +3344,25 @@
         <v>4.3395007995374765E-8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26">
         <f>AVERAGE(B2:B25)</f>
-        <v>1.707385525706276</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.6610716944753685</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27">
         <f>SUM(B2:B25)</f>
-        <v>40.977252616950622</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39.865720667408844</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -3365,7 +3370,7 @@
         <v>1.707385525706276</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3390,14 +3395,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3417,7 +3422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3437,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3457,7 +3462,7 @@
         <v>-0.99524138667034989</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3477,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3485,13 +3490,13 @@
         <v>25027</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3511,7 +3516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -3531,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -3551,7 +3556,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -3571,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -3585,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -3599,7 +3604,7 @@
         <v>2.2644400821123683E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>4.1028703482768693E-2</v>
@@ -3613,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>6.8514938119940277E-2</v>
@@ -3632,14 +3637,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3679,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3699,7 +3704,7 @@
         <v>0.91552133644568556</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3727,13 +3732,13 @@
         <v>14517</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3753,7 +3758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -3793,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -3827,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -3841,7 +3846,7 @@
         <v>7.1366445959230541E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>0.17387237180994605</v>
@@ -3855,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>13.113536832324884</v>
@@ -3874,14 +3879,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3901,7 +3906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>-1.938714303566917</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3961,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3969,13 +3974,13 @@
         <v>22076</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3995,7 +4000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -4015,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -4035,7 +4040,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -4055,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -4069,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -4083,7 +4088,7 @@
         <v>3.7559365872880043E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>0.60788769577183022</v>
@@ -4097,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.74922399674353879</v>
@@ -4116,111 +4121,112 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1.0494704587924837E-9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>-1.9733095580634679</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="15">
+        <v>5.4501942678475027E-9</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>-1.9440395255520231</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1.9332231831124869</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2.2125813604455105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="15">
+        <v>1.598129783659664</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>2.0947214300405346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>-0.69029711616377742</v>
-      </c>
-      <c r="F5">
-        <v>-0.24131894752786978</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="14">
+        <v>-0.82019026632646397</v>
+      </c>
+      <c r="F5" s="14">
+        <v>-0.26052400808039583</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>28996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="15">
+        <v>16449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -4236,12 +4242,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1.7789091219054544E-11</v>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15">
+        <v>8.9972192922551729E-10</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>9</v>
@@ -4256,12 +4262,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>3.0452036718799485E-9</v>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1.5434382787137491E-8</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>10</v>
@@ -4276,12 +4282,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>8.5418613278447627E-11</v>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15">
+        <v>1.6478087179499054E-11</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>11</v>
@@ -4296,21 +4302,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
       </c>
       <c r="F13">
         <f>(F9-F3)^2</f>
-        <v>7.1237969076739344E-4</v>
+        <v>3.1315747004426772E-3</v>
       </c>
       <c r="G13">
         <f>(G9-G3)^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -4321,27 +4327,27 @@
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>4.5190834808864037E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.9721493089238852E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>9.5915876256472771E-2</v>
+        <v>3.2331540323747958E-2</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>1.5408727294916986</v>
+        <v>1.588920774947066</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
-        <v>1.6826918202478027</v>
+        <v>1.6333560392801805</v>
       </c>
     </row>
   </sheetData>
@@ -4357,14 +4363,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4404,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>-0.84012215881109698</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -4452,13 +4458,13 @@
         <v>9140</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -4478,7 +4484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -4498,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -4518,7 +4524,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -4538,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -4552,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -4566,7 +4572,7 @@
         <v>2.5560924103224098E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.10996956868742629</v>
@@ -4580,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.7632158533220309</v>
@@ -4599,14 +4605,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -4646,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -4666,7 +4672,7 @@
         <v>0.97905289583664801</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -4686,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -4694,13 +4700,13 @@
         <v>19855</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -4740,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -4760,7 +4766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -4780,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -4794,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -4808,7 +4814,7 @@
         <v>4.3878117283031837E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.23760718148026433</v>
@@ -4822,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>5.2719812412395459</v>
@@ -4841,14 +4847,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4868,7 +4874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4888,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4908,7 +4914,7 @@
         <v>-0.91426956622166644</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -4928,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -4936,13 +4942,13 @@
         <v>22498</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -4962,7 +4968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -4982,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -5002,7 +5008,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -5022,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -5036,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -5050,7 +5056,7 @@
         <v>7.3497072758212361E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.17340446370532109</v>
@@ -5064,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.36227442272078858</v>
@@ -5083,14 +5089,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5110,7 +5116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5130,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -5150,7 +5156,7 @@
         <v>2.1700843826566474</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -5170,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -5178,13 +5184,13 @@
         <v>39480</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5204,7 +5210,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -5224,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -5244,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -5264,7 +5270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -5278,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -5292,7 +5298,7 @@
         <v>2.8928697223692852E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.50354215896961152</v>
@@ -5306,7 +5312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>5.7217892391712057</v>
@@ -5325,14 +5331,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5352,7 +5358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5372,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5392,7 +5398,7 @@
         <v>-1.9301467610680099</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5412,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5420,12 +5426,12 @@
         <v>6616</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5445,7 +5451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -5465,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -5485,7 +5491,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5505,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -5519,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -5533,7 +5539,7 @@
         <v>4.8794749892897022E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.27491445357257671</v>
@@ -5547,13 +5553,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.53628400644574326</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>45845</v>
       </c>
@@ -5574,14 +5580,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5601,7 +5607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5621,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -5641,7 +5647,7 @@
         <v>-0.93117630681664754</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -5669,13 +5675,13 @@
         <v>20186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5695,7 +5701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -5715,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -5735,7 +5741,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -5755,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -5769,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -5783,7 +5789,7 @@
         <v>4.736700743396236E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>2.1208100339234971E-2</v>
@@ -5797,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.12463458598619642</v>
@@ -5812,18 +5818,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F67123-C238-484A-A862-4793B3762368}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -5834,238 +5840,238 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>8.07</v>
       </c>
       <c r="B2">
         <v>8.0596355951704047E-13</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2">
         <v>0.12463458598619642</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>8.02</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3">
         <v>1.5796560847120545E-12</v>
       </c>
-      <c r="C3" s="12">
-        <v>1.2345762179032729</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="C3" s="11">
+        <v>0.17238004932911505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>8.2100000000000009</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>4.3357871613307814E-12</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4">
         <v>7.3570491299070548E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>8.08</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>1.012008971344051E-11</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5">
         <v>0.53628400644574326</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>8.17</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>3.0307454098484551E-11</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6">
         <v>0.54083169304672596</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>8</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>3.9195619734684774E-11</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7">
         <v>2.2486088556715709</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>8.18</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>4.4799834412673878E-11</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8">
         <v>1.0601366671880055</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>8.1199999999999992</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>4.651193945381306E-11</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9">
         <v>0.7632158533220309</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>8.14</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>5.0178753864547177E-11</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10">
         <v>0.74922399674353879</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11">
         <v>6.7306590467006212E-11</v>
       </c>
       <c r="C11">
         <v>3.0742001074788972</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>8.09</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12">
         <v>7.0465769664118056E-11</v>
       </c>
       <c r="C12">
         <v>5.7217892391712057</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>8.0399999999999991</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>8.0393342108209244E-11</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13">
         <v>6.3703607033352247E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>8.2200000000000006</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14">
         <v>1.1301488435747694E-10</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14">
         <v>2.9872169045337373</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>8.19</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>1.2553290261423606E-10</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15">
         <v>0.22579166495981087</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>8.0500000000000007</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16">
         <v>1.5696951777588024E-10</v>
       </c>
       <c r="C16">
         <v>5.4154243172054854E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>8.1</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17">
         <v>2.8582972675233979E-10</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17">
         <v>0.36227442272078858</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>8.1300000000000008</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18">
         <v>3.724467369690357E-10</v>
       </c>
-      <c r="C18" s="12">
-        <v>1.6826918202478027</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="C18" s="11">
+        <v>1.6333560392801805</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19">
         <v>5.2308606604132552E-10</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19">
         <v>6.0862391056363874E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>8.11</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20">
         <v>7.6460084361251636E-10</v>
       </c>
       <c r="C20">
         <v>5.2719812412395459</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>8.01</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21">
         <v>1.1874474802387587E-9</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21">
         <v>8.3557220422325051E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>8.06</v>
       </c>
       <c r="B22">
         <v>1.5779133853749478E-9</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22">
         <v>0.27286498652861313</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8.15</v>
       </c>
@@ -6076,29 +6082,29 @@
         <v>13.113536832324884</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>8.16</v>
       </c>
       <c r="B24">
         <v>1.1250257867234512E-7</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24">
         <v>6.8514938119940277E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8.23</v>
       </c>
       <c r="B25">
         <v>6.1329098005317547E-7</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25">
         <v>0.6030306303351427</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -6108,12 +6114,12 @@
       </c>
       <c r="C26">
         <f>MEDIAN(C2:C25)</f>
-        <v>0.57193116169093439</v>
+        <v>0.53855784974623466</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
-    <sortCondition ref="B2:B32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
+    <sortCondition ref="B2:B25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6128,14 +6134,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6155,7 +6161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6175,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6195,7 +6201,7 @@
         <v>1.055988293794059</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -6215,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6223,13 +6229,13 @@
         <v>26811</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -6249,7 +6255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6269,7 +6275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -6289,7 +6295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -6309,7 +6315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -6323,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -6337,7 +6343,7 @@
         <v>3.1346890419698663E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0.15748703654128879</v>
@@ -6351,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.27286498652861313</v>
@@ -6370,14 +6376,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6397,7 +6403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6417,7 +6423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6437,7 +6443,7 @@
         <v>2.0693688712303411</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -6457,7 +6463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6465,13 +6471,13 @@
         <v>32931</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -6491,7 +6497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6511,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -6531,7 +6537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -6551,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -6565,7 +6571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -6579,7 +6585,7 @@
         <v>4.8120402957716425E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>1.412636743109587E-3</v>
@@ -6593,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>5.4154243172054854E-2</v>
@@ -6612,14 +6618,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6639,7 +6645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6659,7 +6665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6679,7 +6685,7 @@
         <v>-1.9790612464718986</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -6699,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6707,13 +6713,13 @@
         <v>13648</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -6733,7 +6739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6753,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -6773,7 +6779,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -6793,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -6807,7 +6813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -6821,7 +6827,7 @@
         <v>4.3843139931057769E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>3.1296900840400814E-2</v>
@@ -6835,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>6.3703607033352247E-2</v>
@@ -6854,14 +6860,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6881,7 +6887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6901,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6921,7 +6927,7 @@
         <v>-1.8103587009517974</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -6941,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6949,13 +6955,13 @@
         <v>20520</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -6975,7 +6981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6995,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -7015,7 +7021,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -7035,7 +7041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -7049,7 +7055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -7063,7 +7069,7 @@
         <v>3.5963822304689808E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>5.8291141754522038E-3</v>
@@ -7077,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>6.0862391056363874E-2</v>
@@ -7090,117 +7096,121 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210032DC-5CB8-4BC9-A4C1-B2561DEDF703}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1.4103999578405046E-9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>-1.9979437715596671</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="12">
+        <v>1.1307916401083287E-9</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>-1.9794090510770921</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0.873317977252837</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>-0.89833981807119201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="12">
+        <v>1.0588517580794632</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>-0.89020246593128949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>1.0250913314687904</v>
-      </c>
-      <c r="F5">
-        <v>0.47675026492048783</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1.6517034868941354</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.80355636273399977</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>8676</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="12">
+        <v>10103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -7216,12 +7226,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>3.7491938420104024E-10</v>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1.6896798687566769E-10</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>9</v>
@@ -7236,12 +7246,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>6.3890733762895808E-10</v>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.1175099036090508E-9</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>10</v>
@@ -7256,12 +7266,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>3.2173731516915155E-9</v>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.1058970298402674E-9</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>11</v>
@@ -7276,21 +7286,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
       </c>
       <c r="F13">
         <f>(F9-F3)^2</f>
-        <v>4.2280753988339939E-6</v>
+        <v>4.2398717754580262E-4</v>
       </c>
       <c r="G13">
         <f>(G9-G3)^2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -7301,35 +7311,43 @@
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>1.0334792589798339E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2055498487569646E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.95044691197729592</v>
+        <v>0.12131046104170373</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.2737902852607797</v>
+        <v>3.8590102622295876E-2</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
-        <v>1.2345762179032729</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.17238004932911505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>45847</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>45945</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -7345,14 +7363,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7372,7 +7390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -7392,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -7412,7 +7430,7 @@
         <v>1.9005151978870891</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -7432,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -7440,13 +7458,13 @@
         <v>15895</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -7466,7 +7484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -7486,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -7506,7 +7524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -7526,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f t="shared" ref="E13:G15" si="0">(E9-E3)^2</f>
         <v>0</v>
@@ -7540,7 +7558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7554,7 +7572,7 @@
         <v>9.8972258514450386E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>1.0989139579286872E-2</v>
@@ -7568,7 +7586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>8.3557220422325051E-2</v>
@@ -7587,14 +7605,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7614,7 +7632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7634,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7654,7 +7672,7 @@
         <v>1.0734930225760295</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -7674,7 +7692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7682,12 +7700,12 @@
         <v>12483</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -7707,7 +7725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -7727,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -7747,7 +7765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7767,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f t="shared" ref="E13:G15" si="0">(E9-E3)^2</f>
         <v>0</v>
@@ -7781,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7795,7 +7813,7 @@
         <v>5.4012243673607846E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>2.027326322907663E-4</v>
@@ -7809,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>2.2486088556715709</v>
@@ -7824,18 +7842,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B97CF0-99B2-4337-A953-1577F71FE002}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7855,7 +7873,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -7875,7 +7893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -7895,7 +7913,7 @@
         <v>-0.76266413897423957</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -7915,7 +7933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -7923,13 +7941,13 @@
         <v>18414</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -7949,7 +7967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -7969,7 +7987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -7989,7 +8007,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -8009,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -8023,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -8037,7 +8055,7 @@
         <v>5.6328310928839068E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>0.21056098744513127</v>
@@ -8051,7 +8069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.6030306303351427</v>
@@ -8070,14 +8088,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8097,7 +8115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8117,7 +8135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8137,7 +8155,7 @@
         <v>-1.938860883687646</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8157,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -8165,13 +8183,13 @@
         <v>6348</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -8191,7 +8209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -8211,7 +8229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -8231,7 +8249,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -8251,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -8265,7 +8283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -8279,7 +8297,7 @@
         <v>3.737991543455554E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>2.2622978890600898</v>
@@ -8293,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>2.9872169045337373</v>
@@ -8312,14 +8330,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8339,7 +8357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8359,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8379,7 +8397,7 @@
         <v>1.9955160452234488</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8399,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -8407,13 +8425,13 @@
         <v>16865</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -8433,7 +8451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -8453,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -8473,7 +8491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -8493,7 +8511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -8507,7 +8525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -8521,7 +8539,7 @@
         <v>2.0105850438156042E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>4.2107741416409265E-2</v>
@@ -8535,7 +8553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>7.3570491299070548E-2</v>
@@ -8554,14 +8572,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8581,7 +8599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8601,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8621,7 +8639,7 @@
         <v>1.1588833933359597</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8641,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -8649,13 +8667,13 @@
         <v>16516</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -8675,7 +8693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -8695,7 +8713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -8715,7 +8733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -8735,7 +8753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -8749,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -8763,7 +8781,7 @@
         <v>2.524393267794928E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>9.4606836302567191E-4</v>
@@ -8777,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>3.0742001074788972</v>
@@ -8796,14 +8814,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8823,7 +8841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8843,7 +8861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8863,7 +8881,7 @@
         <v>-1.9546642248812678</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8883,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -8891,13 +8909,13 @@
         <v>9754</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -8917,7 +8935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -8937,7 +8955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -8957,7 +8975,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -8977,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -8991,7 +9009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -9005,7 +9023,7 @@
         <v>2.0553325056162589E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>1.2963273548401879E-2</v>
@@ -9019,7 +9037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.22579166495981087</v>
@@ -9038,14 +9056,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9065,7 +9083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9085,7 +9103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -9105,7 +9123,7 @@
         <v>0.48990804682991446</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -9125,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -9133,13 +9151,13 @@
         <v>34288</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -9159,7 +9177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -9179,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -9199,7 +9217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -9219,7 +9237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -9233,7 +9251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -9247,7 +9265,7 @@
         <v>0.26019380068887282</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>0.7115809718208882</v>
@@ -9261,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>1.0601366671880055</v>
@@ -9280,14 +9298,14 @@
       <selection activeCell="E9" sqref="E9:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9307,7 +9325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9327,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -9347,7 +9365,7 @@
         <v>2.2542873688958283</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -9367,7 +9385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -9375,13 +9393,13 @@
         <v>24059</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -9401,7 +9419,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -9421,7 +9439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -9441,7 +9459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -9461,7 +9479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>(E9-E3)^2</f>
         <v>0</v>
@@ -9475,7 +9493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14">
         <f t="shared" ref="E14:G15" si="0">(E10-E4)^2</f>
         <v>0</v>
@@ -9489,7 +9507,7 @@
         <v>6.4662065979963046E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15">
         <f>(E11-E5)^2</f>
         <v>6.8782620868839501E-3</v>
@@ -9503,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6">
         <f>SUM(E13:G15)</f>
         <v>0.54083169304672596</v>
@@ -9515,20 +9533,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9727,14 +9745,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
@@ -9747,6 +9757,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>